<commit_message>
Finalizo actualizacion septiembre 2020
</commit_message>
<xml_diff>
--- a/MenstruAccion/cuanto_cuesta_menstruar/2020 Septiembre/Fuentes/serie_inflacion.xlsx
+++ b/MenstruAccion/cuanto_cuesta_menstruar/2020 Septiembre/Fuentes/serie_inflacion.xlsx
@@ -232,13 +232,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M7" activeCellId="0" sqref="M7"/>
+      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -448,25 +448,75 @@
       <c r="A15" s="2" t="n">
         <v>43922</v>
       </c>
+      <c r="B15" s="3" t="n">
+        <v>310.1243</v>
+      </c>
+      <c r="C15" s="4" t="n">
+        <v>328.7785</v>
+      </c>
+      <c r="D15" s="4" t="n">
+        <v>337.7523</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
         <v>43952</v>
       </c>
+      <c r="B16" s="3" t="n">
+        <v>314.9087</v>
+      </c>
+      <c r="C16" s="4" t="n">
+        <v>331.0146</v>
+      </c>
+      <c r="D16" s="4" t="n">
+        <v>341.3461</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
         <v>43983</v>
       </c>
+      <c r="B17" s="3" t="n">
+        <v>321.9738</v>
+      </c>
+      <c r="C17" s="4" t="n">
+        <v>334.4636</v>
+      </c>
+      <c r="D17" s="4" t="n">
+        <v>348.9759</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
         <v>44013</v>
       </c>
+      <c r="B18" s="3" t="n">
+        <v>328.2014</v>
+      </c>
+      <c r="C18" s="4" t="n">
+        <v>338.7648</v>
+      </c>
+      <c r="D18" s="4" t="n">
+        <v>356.5467</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
         <v>44044</v>
+      </c>
+      <c r="B19" s="3" t="n">
+        <v>337.0632</v>
+      </c>
+      <c r="C19" s="4" t="n">
+        <v>350.5076</v>
+      </c>
+      <c r="D19" s="4" t="n">
+        <v>365.1113</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="n">
+        <v>44075</v>
       </c>
     </row>
   </sheetData>

</xml_diff>